<commit_message>
Added handling for multiple exchange
</commit_message>
<xml_diff>
--- a/My_Portfolio.xlsx
+++ b/My_Portfolio.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\Data_for_Analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Davidde\Documents\Data_for_Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{179265F1-01DA-4761-B11C-4A4C483CDD4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6A0E232-E64D-40C2-BB96-62132EFF4400}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{78A9643E-E6FF-4F47-A051-AAA42B5BD3AD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{78A9643E-E6FF-4F47-A051-AAA42B5BD3AD}"/>
   </bookViews>
   <sheets>
     <sheet name="My_Portfolio" sheetId="1" r:id="rId1"/>
+    <sheet name="Crypto_Exchanges" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="71">
   <si>
     <t>Symbol</t>
   </si>
@@ -68,15 +69,6 @@
     <t>Category</t>
   </si>
   <si>
-    <t>TR Investment</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TR Shares </t>
-  </si>
-  <si>
-    <t>TR Average Cost</t>
-  </si>
-  <si>
     <t>AMC</t>
   </si>
   <si>
@@ -218,24 +210,52 @@
     <t>Loopring EUR</t>
   </si>
   <si>
-    <t>SOL-USD</t>
-  </si>
-  <si>
-    <t>Solana USD</t>
-  </si>
-  <si>
     <t>USDEUR=X</t>
   </si>
   <si>
     <t>Forex</t>
+  </si>
+  <si>
+    <t>SOL-EUR</t>
+  </si>
+  <si>
+    <t>Solana EUR</t>
+  </si>
+  <si>
+    <t>TR/Crypto.com Investment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TR/Crypto.com Shares </t>
+  </si>
+  <si>
+    <t>TR/Crypto.com Transfer Cost</t>
+  </si>
+  <si>
+    <t>TR/Crypto.com Average Cost After Transfer</t>
+  </si>
+  <si>
+    <t>TR/Crypto.com Average Cost Pre Transfer</t>
+  </si>
+  <si>
+    <t>TR/Crypto.com Share After Transfer</t>
+  </si>
+  <si>
+    <t>BitPanda Commission</t>
+  </si>
+  <si>
+    <t>Crypto Value during Transfer (EUR)</t>
+  </si>
+  <si>
+    <t>Overall Cost Transfer</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="166" formatCode="0.000000"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -714,53 +734,55 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Colore 1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Colore 2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Colore 3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Colore 4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Colore 5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Colore 6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Colore 1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Colore 2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Colore 3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Colore 4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Colore 5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Colore 6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Colore 1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Colore 2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Colore 3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Colore 4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Colore 5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Colore 6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Calcolo" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Cella collegata" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Cella da controllare" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Colore 1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Colore 2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Colore 3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Colore 4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Colore 5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Colore 6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Neutrale" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
-    <cellStyle name="Nota" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Testo avviso" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Testo descrittivo" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Titolo" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Titolo 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Titolo 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Titolo 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Titolo 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Totale" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Valore non valido" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Valore valido" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -776,7 +798,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1092,10 +1114,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECF0E65E-953C-4620-A176-948582FC2C90}">
-  <dimension ref="A1:N25"/>
+  <dimension ref="A1:T25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1108,15 +1130,21 @@
     <col min="6" max="6" width="31.42578125" customWidth="1"/>
     <col min="7" max="7" width="14.7109375" customWidth="1"/>
     <col min="8" max="8" width="19.28515625" customWidth="1"/>
-    <col min="9" max="9" width="24.7109375" customWidth="1"/>
-    <col min="10" max="10" width="22.85546875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="13" customWidth="1"/>
-    <col min="12" max="12" width="17.28515625" customWidth="1"/>
-    <col min="13" max="13" width="23.28515625" customWidth="1"/>
-    <col min="14" max="14" width="13.140625" customWidth="1"/>
+    <col min="9" max="9" width="18.5703125" customWidth="1"/>
+    <col min="10" max="10" width="16" style="1" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" customWidth="1"/>
+    <col min="12" max="12" width="10.5703125" customWidth="1"/>
+    <col min="13" max="13" width="14.42578125" customWidth="1"/>
+    <col min="14" max="14" width="32.28515625" customWidth="1"/>
+    <col min="15" max="15" width="9.42578125" customWidth="1"/>
+    <col min="16" max="16" width="31.28515625" style="2" customWidth="1"/>
+    <col min="17" max="17" width="11.140625" customWidth="1"/>
+    <col min="18" max="18" width="21.85546875" customWidth="1"/>
+    <col min="19" max="19" width="22.85546875" customWidth="1"/>
+    <col min="20" max="20" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1151,21 +1179,39 @@
         <v>10</v>
       </c>
       <c r="L1" t="s">
+        <v>62</v>
+      </c>
+      <c r="M1" t="s">
+        <v>63</v>
+      </c>
+      <c r="N1" t="s">
+        <v>66</v>
+      </c>
+      <c r="O1" t="s">
+        <v>64</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="T1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="B2" t="s">
         <v>12</v>
-      </c>
-      <c r="N1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" t="s">
-        <v>15</v>
       </c>
       <c r="C2">
         <v>36.581949999999999</v>
@@ -1180,24 +1226,26 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>8373.2795769999993</v>
+        <f>SUM($F2:$F24)</f>
+        <v>8485.8795773300008</v>
       </c>
       <c r="I2">
-        <v>29881.182560000001</v>
+        <f>SUM($G2:$G24)</f>
+        <v>30877.170293220479</v>
       </c>
       <c r="J2" s="1">
         <v>45182</v>
       </c>
       <c r="K2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C3">
         <v>257.12049999999999</v>
@@ -1220,15 +1268,15 @@
         <v>45519</v>
       </c>
       <c r="K3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>19</v>
-      </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C4">
         <v>1712.3091999999999</v>
@@ -1249,15 +1297,15 @@
         <v>45517</v>
       </c>
       <c r="K4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C5">
         <v>3.5</v>
@@ -1275,15 +1323,15 @@
         <v>45355</v>
       </c>
       <c r="K5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C6">
         <v>0.29310000000000003</v>
@@ -1301,15 +1349,15 @@
         <v>45355</v>
       </c>
       <c r="K6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C7">
         <v>0.16925999999999999</v>
@@ -1327,15 +1375,15 @@
         <v>45355</v>
       </c>
       <c r="K7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C8">
         <v>0.1191</v>
@@ -1353,15 +1401,15 @@
         <v>45355</v>
       </c>
       <c r="K8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C9">
         <v>0.12903200000000001</v>
@@ -1379,15 +1427,15 @@
         <v>45355</v>
       </c>
       <c r="K9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B10" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C10">
         <v>1.5130300000000001</v>
@@ -1405,15 +1453,15 @@
         <v>45177</v>
       </c>
       <c r="K10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B11" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C11">
         <v>1.032578</v>
@@ -1431,15 +1479,15 @@
         <v>45110</v>
       </c>
       <c r="K11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B12" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C12">
         <v>17.523</v>
@@ -1457,15 +1505,15 @@
         <v>45110</v>
       </c>
       <c r="K12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B13" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C13">
         <f>409+$M13</f>
@@ -1486,7 +1534,7 @@
         <v>45659</v>
       </c>
       <c r="K13" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="L13">
         <f>$M13*$N13</f>
@@ -1499,12 +1547,12 @@
         <v>13.64</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B14" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C14">
         <v>109</v>
@@ -1523,15 +1571,15 @@
         <v>45454</v>
       </c>
       <c r="K14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>42</v>
-      </c>
       <c r="B15" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C15">
         <v>38</v>
@@ -1550,15 +1598,15 @@
         <v>45454</v>
       </c>
       <c r="K15" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B16" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C16">
         <f>$M16</f>
@@ -1579,7 +1627,7 @@
         <v>45659</v>
       </c>
       <c r="K16" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="L16">
         <f>$M16*$N16</f>
@@ -1592,39 +1640,77 @@
         <v>10.130000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B17" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C17">
-        <v>2.0993399999999999E-2</v>
+        <f>$P17</f>
+        <v>1.938724E-2</v>
       </c>
       <c r="E17">
         <f>$G17/$C17</f>
-        <v>33860.594967942307</v>
+        <v>34279.005693078529</v>
       </c>
       <c r="F17">
         <v>0</v>
       </c>
       <c r="G17">
-        <v>710.84901439999999</v>
+        <f>$L17+$S17</f>
+        <v>664.57531033307976</v>
       </c>
       <c r="J17" s="1">
         <v>45349</v>
       </c>
       <c r="K17" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="L17">
+        <f>50.02+25.09+100+100+25+25+(0.99356*48.599793)+47.64+50+50.08+50+50</f>
+        <v>621.11681033308002</v>
+      </c>
+      <c r="M17">
+        <f>0.01984724</f>
+        <v>1.9847239999999999E-2</v>
+      </c>
+      <c r="N17">
+        <f>$L17/$M17</f>
+        <v>31294.870739361246</v>
+      </c>
+      <c r="O17">
+        <f>0.0004</f>
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="P17" s="2">
+        <f>0.01938724</f>
+        <v>1.938724E-2</v>
+      </c>
+      <c r="Q17" s="3">
+        <f>$M17-$O17-$P17</f>
+        <v>5.9999999999997555E-5</v>
+      </c>
+      <c r="R17">
+        <f>94475</f>
+        <v>94475</v>
+      </c>
+      <c r="S17">
+        <f>($O17+$Q17)*$R17</f>
+        <v>43.458499999999773</v>
+      </c>
+      <c r="T17">
+        <f>($L17+$S17)/$P17</f>
+        <v>34279.005693078529</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B18" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C18">
         <v>4.1809430000000002E-2</v>
@@ -1645,15 +1731,15 @@
         <v>45355</v>
       </c>
       <c r="K18" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>51</v>
-      </c>
       <c r="B19" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C19">
         <v>959.39</v>
@@ -1671,15 +1757,15 @@
         <v>44299</v>
       </c>
       <c r="K19" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B20" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C20">
         <v>9.4500000000000001E-2</v>
@@ -1697,15 +1783,15 @@
         <v>44288</v>
       </c>
       <c r="K20" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B21" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C21">
         <v>145.23515</v>
@@ -1726,15 +1812,15 @@
         <v>44288</v>
       </c>
       <c r="K21" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B22" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C22">
         <v>4432927.0199999996</v>
@@ -1755,15 +1841,15 @@
         <v>44357</v>
       </c>
       <c r="K22" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="B23" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C23">
         <v>240.94</v>
@@ -1781,41 +1867,44 @@
         <v>44578</v>
       </c>
       <c r="K23" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>60</v>
+      </c>
+      <c r="B24" t="s">
         <v>61</v>
       </c>
-      <c r="B24" t="s">
-        <v>62</v>
-      </c>
       <c r="C24">
-        <v>0.18679999999999999</v>
+        <f>0.1868+(1.09521322)</f>
+        <v>1.2820132200000001</v>
       </c>
       <c r="E24">
-        <v>133.8621</v>
+        <f>$G24/$C24</f>
+        <v>196.91557445671268</v>
       </c>
       <c r="F24">
         <v>0</v>
       </c>
       <c r="G24">
-        <v>25.005440279999998</v>
+        <f>25.00544028+(($C24-0.1868)*207.67)</f>
+        <v>252.44836967739997</v>
       </c>
       <c r="J24" s="1">
         <v>45355</v>
       </c>
       <c r="K24" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B25" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C25">
         <v>0</v>
@@ -1836,7 +1925,136 @@
         <v>44288</v>
       </c>
       <c r="K25" t="s">
-        <v>64</v>
+        <v>59</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F0FE448-F2B0-4A77-910B-AABB83C7210F}">
+  <dimension ref="A1:H9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="3" width="24.85546875" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" customWidth="1"/>
+    <col min="5" max="5" width="31.28515625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" customWidth="1"/>
+    <col min="7" max="7" width="21.85546875" customWidth="1"/>
+    <col min="8" max="8" width="22.85546875" customWidth="1"/>
+    <col min="9" max="9" width="39" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2">
+        <f>$P2</f>
+        <v>0</v>
+      </c>
+      <c r="F2" s="3"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3">
+        <v>4.1809430000000002E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4">
+        <v>959.39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5">
+        <v>9.4500000000000001E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6">
+        <v>145.23515</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7">
+        <v>4432927.0199999996</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C8">
+        <v>240.94</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C9">
+        <f>0.1868+(1.09521322)</f>
+        <v>1.2820132200000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>